<commit_message>
new file generated based on code changes in APDMAnalysis_v2
</commit_message>
<xml_diff>
--- a/Trial Descriptive Data.xlsx
+++ b/Trial Descriptive Data.xlsx
@@ -17,7 +17,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+  <si>
+    <t>ymean</t>
+  </si>
+  <si>
+    <t>ystd</t>
+  </si>
+  <si>
+    <t>ymin</t>
+  </si>
+  <si>
+    <t>ymax</t>
+  </si>
+  <si>
+    <t>yCV</t>
+  </si>
+  <si>
+    <t>sample_entropy</t>
+  </si>
   <si>
     <t>ymean</t>
   </si>
@@ -165,22 +183,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2">

</xml_diff>